<commit_message>
qa fix to capstatements, update hrex to ver 0.2.0
</commit_message>
<xml_diff>
--- a/input/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
+++ b/input/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Alerts\input\resources\source-data\capstatements-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754B4851-FD9D-4DB3-BE61-32B096C9F2C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00886036-DCFB-4A77-AA55-755878A713C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45915" yWindow="9810" windowWidth="28800" windowHeight="7800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44235" yWindow="8580" windowWidth="28800" windowHeight="7800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="158">
   <si>
     <t>Element</t>
   </si>
@@ -1040,7 +1040,7 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -1810,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1873,7 +1873,7 @@
         <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>104</v>
@@ -1888,7 +1888,7 @@
         <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>116</v>
@@ -1902,7 +1902,7 @@
         <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>101</v>
@@ -1916,7 +1916,7 @@
         <v>154</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>101</v>
@@ -1930,7 +1930,7 @@
         <v>100</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>101</v>
@@ -1944,7 +1944,7 @@
         <v>147</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>102</v>
@@ -1958,7 +1958,7 @@
         <v>148</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>84</v>
@@ -1972,7 +1972,7 @@
         <v>149</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>103</v>
@@ -2099,11 +2099,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:E1048576"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2111,7 +2111,7 @@
     <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
@@ -2239,7 +2239,7 @@
         <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>118</v>
@@ -2250,7 +2250,7 @@
         <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>118</v>
@@ -2261,7 +2261,7 @@
         <v>103</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>118</v>
@@ -2272,7 +2272,7 @@
         <v>105</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>118</v>
@@ -2283,7 +2283,7 @@
         <v>106</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>118</v>
@@ -2294,7 +2294,7 @@
         <v>109</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>118</v>
@@ -2316,7 +2316,7 @@
         <v>108</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>118</v>
@@ -2346,7 +2346,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="77.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
@@ -2401,8 +2401,8 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C17" sqref="C17"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2412,7 +2412,7 @@
     <col min="3" max="3" width="37.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
@@ -2481,6 +2481,27 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
@@ -2501,6 +2522,27 @@
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
@@ -2521,6 +2563,27 @@
       <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
@@ -2541,6 +2604,27 @@
       <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
@@ -2561,6 +2645,27 @@
       <c r="G6" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
@@ -2581,6 +2686,27 @@
       <c r="G7" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
@@ -2601,6 +2727,27 @@
       <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
@@ -2621,6 +2768,27 @@
       <c r="G9" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
@@ -2639,6 +2807,27 @@
         <v>26</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2656,10 +2845,10 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">

</xml_diff>

<commit_message>
fix error in applying FHIR-28357
</commit_message>
<xml_diff>
--- a/input/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
+++ b/input/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Alerts\input\resources\source-data\capstatements-spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-Alerts/input/resources/source-data/capstatements-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00886036-DCFB-4A77-AA55-755878A713C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D876C58-4480-A545-8513-5045B356D37C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44235" yWindow="8580" windowWidth="28800" windowHeight="7800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -33,9 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -567,7 +565,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1040,9 +1038,9 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1050,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>124</v>
       </c>
@@ -1059,7 +1057,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>125</v>
       </c>
@@ -1067,7 +1065,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>126</v>
       </c>
@@ -1075,7 +1073,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -1083,7 +1081,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -1091,7 +1089,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>132</v>
       </c>
@@ -1099,7 +1097,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>134</v>
       </c>
@@ -1123,21 +1121,21 @@
       <selection pane="bottomRight" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
-    <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="68.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -1169,56 +1167,56 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3"/>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4"/>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6"/>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="D9"/>
       <c r="E9"/>
@@ -1226,7 +1224,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10"/>
       <c r="D10"/>
       <c r="E10"/>
@@ -1235,7 +1233,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11"/>
       <c r="D11"/>
       <c r="E11"/>
@@ -1243,14 +1241,14 @@
       <c r="H11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13"/>
       <c r="D13"/>
       <c r="E13"/>
@@ -1258,27 +1256,27 @@
       <c r="H13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17"/>
       <c r="D17"/>
       <c r="E17"/>
@@ -1286,14 +1284,14 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19"/>
       <c r="D19"/>
       <c r="E19"/>
@@ -1302,7 +1300,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20"/>
       <c r="D20"/>
       <c r="E20"/>
@@ -1310,20 +1308,20 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
       <c r="H22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
@@ -1331,7 +1329,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
@@ -1339,7 +1337,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
@@ -1347,25 +1345,25 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:10">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29"/>
       <c r="D29"/>
       <c r="E29"/>
@@ -1374,7 +1372,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:10">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30"/>
       <c r="D30"/>
       <c r="E30"/>
@@ -1383,7 +1381,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31"/>
       <c r="D31"/>
       <c r="E31"/>
@@ -1392,7 +1390,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32"/>
       <c r="D32"/>
       <c r="E32"/>
@@ -1401,203 +1399,203 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="3:10">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="3:10">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="3:10">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="3:10" s="1" customFormat="1">
+    <row r="36" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="3:10">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="3:10" s="1" customFormat="1">
+    <row r="38" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="3:10" s="1" customFormat="1">
+    <row r="39" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="3:10" s="1" customFormat="1">
+    <row r="40" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="41" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H41" s="5"/>
       <c r="I41" s="9"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="42" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H42" s="5"/>
       <c r="I42" s="9"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="3:10" s="1" customFormat="1" ht="15.75">
+    <row r="43" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H43" s="5"/>
       <c r="I43" s="9"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="3:10" s="1" customFormat="1">
+    <row r="44" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="3:10" s="1" customFormat="1">
+    <row r="45" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C45" s="11"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="3:10" s="1" customFormat="1">
+    <row r="46" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C46" s="11"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="3:10" s="1" customFormat="1">
+    <row r="47" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C47" s="11"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="3:10" s="1" customFormat="1">
+    <row r="48" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C48" s="11"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="3:10" s="1" customFormat="1">
+    <row r="49" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C49" s="11"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="3:10" s="1" customFormat="1">
+    <row r="50" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="3:10" s="1" customFormat="1">
+    <row r="51" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="3:10" s="1" customFormat="1">
+    <row r="52" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="3:10" s="1" customFormat="1">
+    <row r="53" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="3:10" s="1" customFormat="1">
+    <row r="54" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="3:10" s="1" customFormat="1">
+    <row r="55" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="3:10" s="1" customFormat="1">
+    <row r="56" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="3:10" s="1" customFormat="1">
+    <row r="57" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="3:10" s="1" customFormat="1">
+    <row r="58" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="3:10" s="1" customFormat="1">
+    <row r="59" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="3:10" s="1" customFormat="1">
+    <row r="60" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="3:10" s="1" customFormat="1">
+    <row r="61" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="3:10" s="1" customFormat="1">
+    <row r="62" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C62" s="11"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="3:10" s="1" customFormat="1">
+    <row r="63" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C63" s="11"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="3:10" s="1" customFormat="1">
+    <row r="64" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="3:16" s="1" customFormat="1">
+    <row r="65" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C65" s="11"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="3:16" s="1" customFormat="1">
+    <row r="66" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C66" s="11"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="3:16" s="1" customFormat="1">
+    <row r="67" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C67" s="11"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="3:16" s="1" customFormat="1">
+    <row r="68" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C68" s="11"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="3:16" s="1" customFormat="1">
+    <row r="69" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="3:16" ht="15.75">
+    <row r="70" spans="3:16" ht="16" x14ac:dyDescent="0.2">
       <c r="C70" s="10"/>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
@@ -1609,62 +1607,62 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="3:16" s="1" customFormat="1">
+    <row r="71" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="3:16" s="1" customFormat="1">
+    <row r="72" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="3:16" s="1" customFormat="1">
+    <row r="73" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="3:16" s="1" customFormat="1">
+    <row r="74" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="3:16" s="1" customFormat="1">
+    <row r="75" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="3:16" s="1" customFormat="1">
+    <row r="76" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="3:16" s="1" customFormat="1">
+    <row r="77" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="3:16" s="1" customFormat="1">
+    <row r="78" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="3:16" s="1" customFormat="1" ht="15.75">
+    <row r="79" spans="3:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H79" s="5"/>
       <c r="I79" s="9"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="3:16" s="1" customFormat="1">
+    <row r="80" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="8:10" s="1" customFormat="1">
+    <row r="81" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="8:10" s="1" customFormat="1">
+    <row r="82" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
@@ -1683,13 +1681,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1697,7 +1695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1705,7 +1703,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
@@ -1713,7 +1711,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
@@ -1721,7 +1719,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105" customHeight="1">
+    <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1729,7 +1727,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1737,7 +1735,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1745,7 +1743,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="207.75" customHeight="1">
+    <row r="8" spans="1:2" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1753,7 +1751,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="103.5" customHeight="1">
+    <row r="9" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1774,12 +1772,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="66.28515625" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1790,7 +1788,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -1814,15 +1812,15 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1836,7 +1834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1851,7 +1849,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>121</v>
       </c>
@@ -1865,7 +1863,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>140</v>
       </c>
@@ -1880,7 +1878,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1">
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>141</v>
       </c>
@@ -1894,7 +1892,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1">
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
@@ -1908,7 +1906,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1">
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>153</v>
       </c>
@@ -1922,7 +1920,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1">
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>123</v>
       </c>
@@ -1936,7 +1934,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1">
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>150</v>
       </c>
@@ -1950,7 +1948,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1">
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>151</v>
       </c>
@@ -1964,7 +1962,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1">
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -1978,7 +1976,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1">
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f t="shared" ref="A12:A16" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(D12)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
@@ -1994,7 +1992,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1">
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f t="shared" ref="A13" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(D13)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
@@ -2010,7 +2008,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1">
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
@@ -2026,7 +2024,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1">
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
@@ -2042,7 +2040,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1">
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
@@ -2058,35 +2056,35 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F26" s="1"/>
     </row>
   </sheetData>
@@ -2103,26 +2101,26 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="14" width="17.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" style="1" customWidth="1"/>
-    <col min="16" max="19" width="17.42578125" style="1" customWidth="1"/>
-    <col min="20" max="21" width="20.42578125" style="1" customWidth="1"/>
-    <col min="22" max="25" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="17.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" style="1" customWidth="1"/>
+    <col min="16" max="19" width="17.5" style="1" customWidth="1"/>
+    <col min="20" max="21" width="20.5" style="1" customWidth="1"/>
+    <col min="22" max="25" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" thickBot="1">
+    <row r="1" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2199,7 +2197,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15.75" thickTop="1">
+    <row r="2" spans="1:25" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
@@ -2207,7 +2205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -2215,7 +2213,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>142</v>
       </c>
@@ -2223,7 +2221,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="1" customFormat="1">
+    <row r="5" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>143</v>
       </c>
@@ -2234,7 +2232,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:25" ht="45">
+    <row r="6" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>102</v>
       </c>
@@ -2245,7 +2243,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="45">
+    <row r="7" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
@@ -2256,7 +2254,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="45">
+    <row r="8" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>103</v>
       </c>
@@ -2267,7 +2265,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="45">
+    <row r="9" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>105</v>
       </c>
@@ -2278,7 +2276,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="45">
+    <row r="10" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>106</v>
       </c>
@@ -2289,7 +2287,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="45">
+    <row r="11" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>109</v>
       </c>
@@ -2300,34 +2298,34 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="45">
+    <row r="12" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="45">
+    <row r="13" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="22:25" ht="18">
+    <row r="36" spans="22:25" ht="18" x14ac:dyDescent="0.2">
       <c r="V36" s="7"/>
       <c r="X36" s="7"/>
       <c r="Y36" s="7"/>
     </row>
-    <row r="39" spans="22:25" ht="18">
+    <row r="39" spans="22:25" ht="18" x14ac:dyDescent="0.2">
       <c r="Y39" s="7"/>
     </row>
   </sheetData>
@@ -2344,16 +2342,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="77.5" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2370,7 +2368,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>119</v>
       </c>
@@ -2387,7 +2385,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -2405,20 +2403,20 @@
       <selection pane="topRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2462,7 +2460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2503,7 +2501,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2544,7 +2542,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2585,7 +2583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2626,7 +2624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2667,7 +2665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2708,7 +2706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2749,7 +2747,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2790,7 +2788,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -2845,13 +2843,13 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2863,7 +2861,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C2" s="2"/>
       <c r="G2" s="2"/>
     </row>
@@ -2883,34 +2881,34 @@
       <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.7109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
+    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.7109375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.140625" customWidth="1"/>
+    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18.95" customHeight="1" thickBot="1">
+    <row r="1" spans="1:28" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -2996,29 +2994,29 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1" thickTop="1">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="12"/>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
       <c r="AA3" s="12"/>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA4" s="12"/>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z5" s="5"/>
       <c r="AA5" s="12"/>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="6" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="12"/>
     </row>
-    <row r="7" spans="1:28" ht="18.95" customHeight="1">
+    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="C7" s="6"/>
       <c r="E7"/>
@@ -3028,7 +3026,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="12"/>
     </row>
-    <row r="8" spans="1:28" ht="18.95" customHeight="1">
+    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8"/>
       <c r="C8"/>
       <c r="E8"/>
@@ -3037,7 +3035,7 @@
       <c r="AA8" s="12"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" ht="18.95" customHeight="1">
+    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9"/>
       <c r="E9"/>
@@ -3048,7 +3046,7 @@
       <c r="AA9" s="12"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" ht="18.95" customHeight="1">
+    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10"/>
       <c r="D10"/>
       <c r="E10"/>
@@ -3064,7 +3062,7 @@
       <c r="AA10" s="12"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" ht="18.95" customHeight="1">
+    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11"/>
       <c r="C11"/>
       <c r="E11"/>
@@ -3076,7 +3074,7 @@
       <c r="AA11" s="12"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" ht="18.95" customHeight="1">
+    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12"/>
       <c r="C12"/>
       <c r="E12"/>
@@ -3084,7 +3082,7 @@
       <c r="AA12" s="12"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="18.95" customHeight="1">
+    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
@@ -3094,7 +3092,7 @@
       <c r="AA13" s="12"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="18.95" customHeight="1">
+    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
@@ -3104,12 +3102,12 @@
       <c r="Z14" s="5"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
       <c r="AA15" s="12"/>
     </row>
-    <row r="16" spans="1:28" ht="18.95" customHeight="1">
+    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16"/>
       <c r="C16"/>
       <c r="E16"/>
@@ -3117,7 +3115,7 @@
       <c r="AA16" s="12"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="2:28" ht="18.95" customHeight="1">
+    <row r="17" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
@@ -3128,7 +3126,7 @@
       <c r="AA17" s="12"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="2:28" ht="18.95" customHeight="1">
+    <row r="18" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
@@ -3139,7 +3137,7 @@
       <c r="AA18" s="12"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="2:28" ht="18.95" customHeight="1">
+    <row r="19" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19"/>
       <c r="C19"/>
       <c r="J19"/>
@@ -3149,7 +3147,7 @@
       <c r="AA19" s="12"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="2:28" ht="18.95" customHeight="1">
+    <row r="20" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20"/>
       <c r="C20"/>
       <c r="X20"/>
@@ -3158,7 +3156,7 @@
       <c r="AA20" s="12"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="2:28" ht="18.95" customHeight="1">
+    <row r="21" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
@@ -3167,21 +3165,21 @@
       <c r="Z21" s="5"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="2:28" ht="18.95" customHeight="1">
+    <row r="22" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22"/>
       <c r="C22"/>
       <c r="E22"/>
       <c r="Z22"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="2:28" ht="18.95" customHeight="1">
+    <row r="23" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23"/>
       <c r="E23"/>
       <c r="J23" s="6"/>
       <c r="Y23"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="2:28" ht="18.95" customHeight="1">
+    <row r="24" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24"/>
       <c r="C24"/>
       <c r="E24"/>
@@ -3190,7 +3188,7 @@
       <c r="AA24" s="12"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="2:28" ht="18.95" customHeight="1">
+    <row r="25" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25"/>
       <c r="C25"/>
       <c r="E25"/>
@@ -3198,7 +3196,7 @@
       <c r="AA25" s="12"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="2:28" ht="18.95" customHeight="1">
+    <row r="26" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -3209,7 +3207,7 @@
       <c r="AA26" s="12"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="2:28" ht="18.95" customHeight="1">
+    <row r="27" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -3221,304 +3219,304 @@
       <c r="AA27" s="12"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="2:28" ht="18.95" customHeight="1">
+    <row r="28" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28"/>
       <c r="C28"/>
       <c r="J28"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="2:28" ht="18.95" customHeight="1">
+    <row r="29" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29"/>
       <c r="J29"/>
       <c r="X29"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="2:28" ht="18.95" customHeight="1">
+    <row r="30" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30"/>
       <c r="J30"/>
       <c r="X30"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="2:28" ht="18.95" customHeight="1">
+    <row r="31" spans="2:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31"/>
       <c r="J31"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="2:28" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="32" spans="2:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="33" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="34" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="35" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA35" s="12"/>
     </row>
-    <row r="36" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="36" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
       <c r="AA36" s="12"/>
     </row>
-    <row r="37" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="37" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z37" s="5"/>
       <c r="AA37" s="12"/>
     </row>
-    <row r="38" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="38" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
       <c r="AA38" s="12"/>
     </row>
-    <row r="39" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="39" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA39" s="12"/>
     </row>
-    <row r="40" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="40" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
       <c r="AA40" s="2"/>
     </row>
-    <row r="41" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="41" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
       <c r="AA41" s="12"/>
     </row>
-    <row r="42" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="42" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z42" s="5"/>
       <c r="AA42" s="12"/>
     </row>
-    <row r="43" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="43" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
       <c r="AA43" s="12"/>
     </row>
-    <row r="44" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="44" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
       <c r="AA44" s="12"/>
     </row>
-    <row r="45" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="45" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA45" s="12"/>
     </row>
-    <row r="46" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="46" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA46" s="12"/>
     </row>
-    <row r="47" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="47" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
       <c r="AA47" s="12"/>
     </row>
-    <row r="48" spans="25:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="48" spans="25:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z48" s="5"/>
       <c r="AA48" s="12"/>
     </row>
-    <row r="49" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="49" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
       <c r="AA49" s="12"/>
     </row>
-    <row r="50" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="50" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
       <c r="AA50" s="12"/>
     </row>
-    <row r="51" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="51" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N51" s="14"/>
       <c r="AA51" s="12"/>
     </row>
-    <row r="52" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="52" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y52" s="5"/>
       <c r="Z52" s="5"/>
       <c r="AA52" s="12"/>
     </row>
-    <row r="53" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="53" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z53" s="5"/>
       <c r="AA53" s="12"/>
     </row>
-    <row r="54" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="54" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA54" s="12"/>
     </row>
-    <row r="55" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="55" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
       <c r="AA55" s="12"/>
     </row>
-    <row r="56" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="56" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="U56" s="7"/>
       <c r="V56" s="7"/>
       <c r="Z56" s="12"/>
       <c r="AA56" s="12"/>
     </row>
-    <row r="57" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="57" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA57" s="12"/>
     </row>
-    <row r="58" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="58" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y58" s="5"/>
       <c r="Z58" s="5"/>
       <c r="AA58" s="12"/>
     </row>
-    <row r="59" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="59" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V59" s="7"/>
       <c r="Z59" s="12"/>
       <c r="AA59" s="12"/>
     </row>
-    <row r="60" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="60" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N60" s="14"/>
       <c r="AA60" s="12"/>
     </row>
-    <row r="61" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="61" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y61" s="5"/>
       <c r="Z61" s="5"/>
       <c r="AA61" s="12"/>
     </row>
-    <row r="62" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="62" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z62" s="5"/>
       <c r="AA62" s="12"/>
     </row>
-    <row r="63" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="63" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA63" s="12"/>
     </row>
-    <row r="64" spans="14:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="64" spans="14:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y64" s="5"/>
       <c r="Z64" s="5"/>
       <c r="AA64" s="12"/>
     </row>
-    <row r="65" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="65" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y65" s="5"/>
       <c r="Z65" s="5"/>
       <c r="AA65" s="12"/>
     </row>
-    <row r="66" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="66" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y66" s="5"/>
       <c r="Z66" s="5"/>
       <c r="AA66" s="12"/>
     </row>
-    <row r="67" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="67" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y67" s="5"/>
       <c r="Z67" s="5"/>
       <c r="AA67" s="12"/>
     </row>
-    <row r="68" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="68" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA68" s="12"/>
     </row>
-    <row r="69" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="69" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z69" s="5"/>
       <c r="AA69" s="12"/>
     </row>
-    <row r="70" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="70" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y70" s="5"/>
       <c r="Z70" s="5"/>
       <c r="AA70" s="12"/>
     </row>
-    <row r="71" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="71" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y71" s="5"/>
       <c r="Z71" s="5"/>
       <c r="AA71" s="12"/>
     </row>
-    <row r="72" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="72" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA72" s="12"/>
     </row>
-    <row r="73" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="73" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z73" s="5"/>
       <c r="AA73" s="12"/>
     </row>
-    <row r="74" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="74" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y74" s="5"/>
       <c r="Z74" s="5"/>
       <c r="AA74" s="12"/>
     </row>
-    <row r="75" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="75" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z75" s="5"/>
       <c r="AA75" s="12"/>
     </row>
-    <row r="76" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="76" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y76" s="5"/>
       <c r="Z76" s="5"/>
       <c r="AA76" s="12"/>
     </row>
-    <row r="77" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="77" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z77" s="5"/>
       <c r="AA77" s="12"/>
     </row>
-    <row r="78" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="78" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z78" s="5"/>
       <c r="AA78" s="12"/>
     </row>
-    <row r="79" spans="7:27" ht="18.95" customHeight="1">
+    <row r="79" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="Z79" s="7"/>
       <c r="AA79" s="12"/>
     </row>
-    <row r="80" spans="7:27" ht="18.95" customHeight="1">
+    <row r="80" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="Z80" s="7"/>
       <c r="AA80" s="12"/>
     </row>
-    <row r="81" spans="7:27" ht="18.95" customHeight="1">
+    <row r="81" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="Z81" s="7"/>
       <c r="AA81" s="12"/>
     </row>
-    <row r="82" spans="7:27" ht="18.95" customHeight="1">
+    <row r="82" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="Z82" s="7"/>
       <c r="AA82" s="12"/>
     </row>
-    <row r="83" spans="7:27" ht="18.95" customHeight="1">
+    <row r="83" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="Z83" s="7"/>
       <c r="AA83" s="12"/>
     </row>
-    <row r="84" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="84" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z84" s="7"/>
       <c r="AA84" s="12"/>
     </row>
-    <row r="85" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="85" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z85" s="7"/>
       <c r="AA85" s="12"/>
     </row>
-    <row r="86" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="86" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z86" s="7"/>
       <c r="AA86" s="12"/>
     </row>
-    <row r="87" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="87" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z87" s="7"/>
       <c r="AA87" s="12"/>
     </row>
-    <row r="88" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="88" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z88" s="7"/>
       <c r="AA88" s="12"/>
     </row>
-    <row r="89" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="89" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y89" s="5"/>
       <c r="Z89" s="7"/>
       <c r="AA89" s="12"/>
     </row>
-    <row r="90" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="90" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y90" s="5"/>
       <c r="Z90" s="7"/>
       <c r="AA90" s="12"/>
     </row>
-    <row r="91" spans="7:27" s="1" customFormat="1" ht="18.95" customHeight="1">
+    <row r="91" spans="7:27" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y91" s="5"/>
       <c r="Z91" s="7"/>
       <c r="AA91" s="12"/>
     </row>
-    <row r="92" spans="7:27" ht="18.95" customHeight="1">
+    <row r="92" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y92" s="5"/>
       <c r="Z92" s="7"/>
       <c r="AA92" s="12"/>
     </row>
-    <row r="93" spans="7:27" ht="18.95" customHeight="1">
+    <row r="93" spans="7:27" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y93" s="5"/>
     </row>
   </sheetData>

</xml_diff>